<commit_message>
edit v ll_grammar.xlsx id na func_id, v parser.c podpora func_id + argument sem_type v cmp_type(), ve scanner.c podpora func_id. added semantic.c semantic.h
</commit_message>
<xml_diff>
--- a/doc/ll_grammar.xlsx
+++ b/doc/ll_grammar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programovani\VUT\BIT2\IFJ\compilerIFJ23\ifj-projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72573E16-0B1A-4202-8CC8-21C60FD68157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80487397-99B6-47BF-82D4-6081B6FFEB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E1A4EF7F-483A-4F6F-9272-5E87C3ECC0F0}"/>
   </bookViews>
@@ -134,9 +134,6 @@
     <t>FUNC_STMT_LIST</t>
   </si>
   <si>
-    <t>func id ( P_LIST ) RET_TYPE { FUNC_STMT_LIST }</t>
-  </si>
-  <si>
     <t>FUNC_STMT</t>
   </si>
   <si>
@@ -228,6 +225,9 @@
   </si>
   <si>
     <t>return EXP</t>
+  </si>
+  <si>
+    <t>func func_id ( P_LIST ) RET_TYPE { FUNC_STMT_LIST }</t>
   </si>
 </sst>
 </file>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9835BFAF-D074-4BDD-982D-B1F687DAD0F9}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
         <v>::=</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
@@ -618,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B64" si="0">$I$2</f>
+        <f t="shared" ref="B2:B59" si="0">$I$2</f>
         <v>::=</v>
       </c>
       <c r="C2" t="str">
@@ -626,7 +626,7 @@
         <v>''</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -686,7 +686,7 @@
         <v>::=</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
         <v>::=</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>::=</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -972,7 +972,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
@@ -984,91 +984,91 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C32" t="s">
         <v>33</v>
-      </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C32" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
@@ -1081,38 +1081,38 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C40" t="s">
         <v>39</v>
-      </c>
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C40" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C42" t="s">
         <v>41</v>
-      </c>
-      <c r="B42" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C42" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1124,24 +1124,24 @@
         <v>::=</v>
       </c>
       <c r="C43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C44" t="s">
         <v>44</v>
-      </c>
-      <c r="B44" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C44" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
@@ -1166,14 +1166,14 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C47" t="s">
         <v>46</v>
-      </c>
-      <c r="B47" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C47" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1185,36 +1185,36 @@
         <v>::=</v>
       </c>
       <c r="C48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C49" t="s">
         <v>51</v>
-      </c>
-      <c r="B49" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C49" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
@@ -1226,14 +1226,14 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C52" t="s">
         <v>56</v>
-      </c>
-      <c r="B52" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C52" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
         <v>::=</v>
       </c>
       <c r="C53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>::=</v>
       </c>
       <c r="C54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1269,7 +1269,7 @@
         <v>::=</v>
       </c>
       <c r="C55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1281,7 +1281,7 @@
         <v>::=</v>
       </c>
       <c r="C56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1293,7 +1293,7 @@
         <v>::=</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1305,7 +1305,7 @@
         <v>::=</v>
       </c>
       <c r="C58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1317,7 +1317,7 @@
         <v>::=</v>
       </c>
       <c r="C59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit v parser.c = exp misto R_RIGID. added some more semantic rules
</commit_message>
<xml_diff>
--- a/doc/ll_grammar.xlsx
+++ b/doc/ll_grammar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programovani\VUT\BIT2\IFJ\compilerIFJ23\ifj-projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80487397-99B6-47BF-82D4-6081B6FFEB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC835F6E-9D1F-49CE-827D-C48D45D43272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E1A4EF7F-483A-4F6F-9272-5E87C3ECC0F0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
   <si>
     <t>''</t>
   </si>
@@ -586,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9835BFAF-D074-4BDD-982D-B1F687DAD0F9}">
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B59" si="0">$I$2</f>
+        <f t="shared" ref="B2:B58" si="0">$I$2</f>
         <v>::=</v>
       </c>
       <c r="C2" t="str">
@@ -763,14 +763,14 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
+      <c r="C14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>::=</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -794,7 +794,7 @@
         <v>::=</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -806,19 +806,20 @@
         <v>::=</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C18" t="s">
-        <v>22</v>
+      <c r="C18" t="str">
+        <f xml:space="preserve"> I1</f>
+        <v>''</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -829,33 +830,32 @@
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C19" t="str">
-        <f xml:space="preserve"> I1</f>
-        <v>''</v>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>17</v>
+      <c r="C20" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -866,33 +866,34 @@
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C22" t="s">
-        <v>25</v>
+      <c r="C22" t="str">
+        <f xml:space="preserve"> I1</f>
+        <v>''</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C23" t="str">
-        <f xml:space="preserve"> I1</f>
-        <v>''</v>
+      <c r="C23" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C24" t="s">
-        <v>27</v>
+      <c r="C24" t="str">
+        <f>I1</f>
+        <v>''</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -903,21 +904,21 @@
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C25" t="str">
-        <f>I1</f>
-        <v>''</v>
+      <c r="C25" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C26" t="s">
-        <v>28</v>
+      <c r="C26" t="str">
+        <f xml:space="preserve"> I1</f>
+        <v>''</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -928,21 +929,20 @@
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C27" t="str">
-        <f xml:space="preserve"> I1</f>
-        <v>''</v>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>30</v>
+      <c r="C28" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -953,21 +953,21 @@
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C29" t="s">
-        <v>49</v>
+      <c r="C29" t="str">
+        <f>I1</f>
+        <v>''</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C30" t="str">
-        <f>I1</f>
-        <v>''</v>
+      <c r="C30" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -979,7 +979,7 @@
         <v>::=</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,7 +991,7 @@
         <v>::=</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1003,7 +1003,7 @@
         <v>::=</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1015,55 +1015,56 @@
         <v>::=</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C38" t="s">
-        <v>37</v>
+      <c r="C38" t="str">
+        <f>I1</f>
+        <v>''</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1074,21 +1075,20 @@
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C39" t="str">
-        <f>I1</f>
-        <v>''</v>
+      <c r="C39" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1100,31 +1100,31 @@
         <v>::=</v>
       </c>
       <c r="C41" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C43" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1135,21 +1135,21 @@
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C44" t="s">
-        <v>44</v>
+      <c r="C44" t="str">
+        <f>I1</f>
+        <v>''</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C45" t="str">
-        <f>I1</f>
-        <v>''</v>
+      <c r="C45" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1161,43 +1161,43 @@
         <v>::=</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C49" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1208,32 +1208,32 @@
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C50" t="s">
-        <v>55</v>
+      <c r="C50" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>17</v>
+      <c r="C51" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C52" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
         <v>::=</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>::=</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1269,7 +1269,7 @@
         <v>::=</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1281,7 +1281,7 @@
         <v>::=</v>
       </c>
       <c r="C56" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1293,7 +1293,7 @@
         <v>::=</v>
       </c>
       <c r="C57" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1305,18 +1305,6 @@
         <v>::=</v>
       </c>
       <c r="C58" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C59" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add: if let id
</commit_message>
<xml_diff>
--- a/doc/ll_grammar.xlsx
+++ b/doc/ll_grammar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programovani\VUT\BIT2\IFJ\compilerIFJ23\ifj-projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC835F6E-9D1F-49CE-827D-C48D45D43272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B68F93B-B76B-4BE8-A3E2-133E442B1FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E1A4EF7F-483A-4F6F-9272-5E87C3ECC0F0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="70">
   <si>
     <t>''</t>
   </si>
@@ -149,9 +149,6 @@
     <t>while EXP { FUNC_STMT_LIST }</t>
   </si>
   <si>
-    <t>if EXP { FUNC_STMT_LIST } FUNC_ELSE_CLAUSE</t>
-  </si>
-  <si>
     <t>FUNC_ELSE_CLAUSE</t>
   </si>
   <si>
@@ -164,9 +161,6 @@
     <t>{ FUNC_STMT_LIST }</t>
   </si>
   <si>
-    <t>if EXP { STMT_LIST } ELSE_CLAUSE</t>
-  </si>
-  <si>
     <t>ELSE_CLAUSE</t>
   </si>
   <si>
@@ -228,6 +222,30 @@
   </si>
   <si>
     <t>func func_id ( P_LIST ) RET_TYPE { FUNC_STMT_LIST }</t>
+  </si>
+  <si>
+    <t>IF_COND</t>
+  </si>
+  <si>
+    <t>let id</t>
+  </si>
+  <si>
+    <t>if IF_COND { FUNC_STMT_LIST } FUNC_ELSE_CLAUSE</t>
+  </si>
+  <si>
+    <t>if IF_COND { STMT_LIST } ELSE_CLAUSE</t>
+  </si>
+  <si>
+    <t>Bool_Ni</t>
+  </si>
+  <si>
+    <t>Double_Nil</t>
+  </si>
+  <si>
+    <t>Int_Nil</t>
+  </si>
+  <si>
+    <t>String_Nil</t>
   </si>
 </sst>
 </file>
@@ -586,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9835BFAF-D074-4BDD-982D-B1F687DAD0F9}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +625,7 @@
         <v>::=</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
@@ -618,7 +636,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B58" si="0">$I$2</f>
+        <f t="shared" ref="B2:B64" si="0">$I$2</f>
         <v>::=</v>
       </c>
       <c r="C2" t="str">
@@ -626,7 +644,7 @@
         <v>''</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -686,7 +704,7 @@
         <v>::=</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -811,56 +829,55 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C18" t="str">
-        <f xml:space="preserve"> I1</f>
-        <v>''</v>
+      <c r="C18" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>17</v>
+      <c r="C19" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -873,44 +890,43 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C23" t="s">
-        <v>27</v>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C24" t="str">
-        <f>I1</f>
-        <v>''</v>
+      <c r="C24" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
@@ -923,87 +939,89 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>30</v>
+      <c r="C27" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C28" t="s">
-        <v>49</v>
+      <c r="C28" t="str">
+        <f>I1</f>
+        <v>''</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C30" t="str">
+        <f xml:space="preserve"> I1</f>
+        <v>''</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C29" t="str">
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C33" t="str">
         <f>I1</f>
         <v>''</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C33" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1015,261 +1033,261 @@
         <v>::=</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C35" t="s">
         <v>33</v>
-      </c>
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C35" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C36" t="s">
         <v>34</v>
-      </c>
-      <c r="B36" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C36" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C38" t="str">
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C42" t="str">
         <f>I1</f>
         <v>''</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C42" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C44" t="str">
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C48" t="str">
         <f>I1</f>
         <v>''</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B47" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C48" t="s">
-        <v>51</v>
-      </c>
-    </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>17</v>
+      <c r="C50" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C51" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C52" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C53" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
-      <c r="C54" t="s">
-        <v>58</v>
+      <c r="C54" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
         <v>::=</v>
       </c>
       <c r="C55" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1281,7 +1299,7 @@
         <v>::=</v>
       </c>
       <c r="C56" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1293,7 +1311,7 @@
         <v>::=</v>
       </c>
       <c r="C57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1305,7 +1323,79 @@
         <v>::=</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C61" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C64" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: commentary, modified: doc/ll_diagram.png, doc/ll_grammar.xlsx
</commit_message>
<xml_diff>
--- a/doc/ll_grammar.xlsx
+++ b/doc/ll_grammar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programovani\VUT\BIT2\IFJ\compilerIFJ23\ifj-projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD829F03-F0F9-4A2A-BC9C-7E06016BA7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52229861-CEB6-4AD4-948D-A4012D0CDC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E1A4EF7F-483A-4F6F-9272-5E87C3ECC0F0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="75">
   <si>
     <t>''</t>
   </si>
@@ -170,12 +170,6 @@
     <t>AFTER_ELSE</t>
   </si>
   <si>
-    <t>{ STMT_LIST }</t>
-  </si>
-  <si>
-    <t>while EXP { STMT_LIST }</t>
-  </si>
-  <si>
     <t>STMT_LIST eof</t>
   </si>
   <si>
@@ -224,9 +218,6 @@
     <t>if IF_COND { FUNC_STMT_LIST } FUNC_ELSE_CLAUSE</t>
   </si>
   <si>
-    <t>if IF_COND { STMT_LIST } ELSE_CLAUSE</t>
-  </si>
-  <si>
     <t>Bool_Ni</t>
   </si>
   <si>
@@ -243,13 +234,40 @@
   </si>
   <si>
     <t>func_id</t>
+  </si>
+  <si>
+    <t>LOCAL_STMT_LIST</t>
+  </si>
+  <si>
+    <t>LOCAL_STMT LOCAL_STMT_LIST</t>
+  </si>
+  <si>
+    <t>LOCAL_STMT</t>
+  </si>
+  <si>
+    <t>{ LOCAL_STMT_LIST }</t>
+  </si>
+  <si>
+    <t>while EXP { LOCAL_STMT_LIST }</t>
+  </si>
+  <si>
+    <t>if IF_COND { LOCAL_STMT_LIST } ELSE_CLAUSE</t>
+  </si>
+  <si>
+    <t>FUNC_ELSE_IF</t>
+  </si>
+  <si>
+    <t>ELSE_IF_STMT</t>
+  </si>
+  <si>
+    <t>if EXP { LOCAL_STMT_LIST } ELSE_CLAUSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +280,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -284,9 +314,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,774 +635,873 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9835BFAF-D074-4BDD-982D-B1F687DAD0F9}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="55.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1" s="1" t="str">
         <f>$I$2</f>
         <v>::=</v>
       </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="str">
-        <f t="shared" ref="B2:B62" si="0">$I$2</f>
-        <v>::=</v>
-      </c>
-      <c r="C2" t="str">
+      <c r="B2" s="1" t="str">
+        <f t="shared" ref="B2:B65" si="0">$I$2</f>
+        <v>::=</v>
+      </c>
+      <c r="C2" s="1" t="str">
         <f>I1</f>
         <v>''</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>50</v>
+      <c r="I2" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
+      <c r="B7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C21" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C22" t="str">
+      <c r="B22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C22" s="1" t="str">
         <f xml:space="preserve"> I1</f>
         <v>''</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B24" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C24" t="s">
-        <v>58</v>
+      <c r="B24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C26" t="str">
+      <c r="B26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C26" s="1" t="str">
         <f xml:space="preserve"> I1</f>
         <v>''</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C28" t="str">
+      <c r="B28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C28" s="1" t="str">
         <f>I1</f>
         <v>''</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C30" t="str">
+      <c r="B30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C30" s="1" t="str">
         <f xml:space="preserve"> I1</f>
         <v>''</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C32" t="s">
-        <v>47</v>
+      <c r="B32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C33" t="str">
+      <c r="B33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C33" s="1" t="str">
         <f>I1</f>
         <v>''</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B36" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B37" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C37" t="s">
-        <v>48</v>
+      <c r="B37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B38" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B39" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C39" t="s">
-        <v>57</v>
+      <c r="B39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B41" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C41" t="s">
-        <v>61</v>
+      <c r="B41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B42" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C42" t="str">
+      <c r="B42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C42" s="1" t="str">
         <f>I1</f>
         <v>''</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B43" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B44" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C44" t="s">
-        <v>35</v>
+      <c r="B44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B45" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="B45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B46" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C46" t="s">
-        <v>62</v>
+      <c r="B46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B47" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B48" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C48" t="str">
+      <c r="B48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C48" s="1" t="str">
         <f>I1</f>
         <v>''</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B49" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="B49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C64" s="1" t="str">
+        <f>I1</f>
+        <v>''</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>::=</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="1" t="str">
+        <f t="shared" ref="B66:B70" si="1">$I$2</f>
+        <v>::=</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>::=</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C50" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>::=</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B51" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C51" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>48</v>
-      </c>
-      <c r="B52" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C52" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>7</v>
-      </c>
-      <c r="B54" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C54" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>7</v>
-      </c>
-      <c r="B55" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C55" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>7</v>
-      </c>
-      <c r="B56" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C56" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>7</v>
-      </c>
-      <c r="B57" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C57" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>7</v>
-      </c>
-      <c r="B58" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C58" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C59" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>7</v>
-      </c>
-      <c r="B60" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C60" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>::=</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B61" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62" t="str">
-        <f t="shared" si="0"/>
-        <v>::=</v>
-      </c>
-      <c r="C62" t="s">
-        <v>60</v>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>::=</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>